<commit_message>
feat(): Introduce automatically generated overview of findings (in technical details section)
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -22,7 +22,7 @@
     <t>Author: Lauritz Holtmann</t>
   </si>
   <si>
-    <t>Date: 2022-09-28</t>
+    <t>Date: 2023-03-23</t>
   </si>
   <si>
     <t>Finding-ID</t>
@@ -37,7 +37,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>#PEN20220001</t>
+    <t>#PEN20230001</t>
   </si>
   <si>
     <t>Critical (9.1)</t>
@@ -49,7 +49,7 @@
     <t>XXE in Test Shop</t>
   </si>
   <si>
-    <t>#PEN20220002</t>
+    <t>#PEN20230002</t>
   </si>
   <si>
     <t>High (7.1)</t>

</xml_diff>

<commit_message>
feat(): Visual adjustments and addition of further example finding
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Pentest Report: Example Report</t>
   </si>
@@ -56,6 +56,15 @@
   </si>
   <si>
     <t>XSS in Test Shop</t>
+  </si>
+  <si>
+    <t>#PEN20230003</t>
+  </si>
+  <si>
+    <t>Low (3.1)</t>
+  </si>
+  <si>
+    <t>Open Redirect in Test Shop</t>
   </si>
 </sst>
 </file>
@@ -403,7 +412,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -466,6 +475,20 @@
         <v>13</v>
       </c>
     </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>